<commit_message>
Filled out 9d lost muon fits that I didn't have in the table.
</commit_message>
<xml_diff>
--- a/OtherMaterials/LostMuonRComparison.xlsx
+++ b/OtherMaterials/LostMuonRComparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C403C5-C9B3-DC4D-99DA-CEC685984D57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03BE511-2282-774D-96F4-97E2826137CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39120" yWindow="19720" windowWidth="22900" windowHeight="16460" xr2:uid="{391225D3-A562-3048-83E8-B4C713E70867}"/>
+    <workbookView xWindow="3520" yWindow="1800" windowWidth="24820" windowHeight="17580" xr2:uid="{391225D3-A562-3048-83E8-B4C713E70867}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>new histogram, base cuts</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>9d</t>
+  </si>
+  <si>
+    <t>main cuts with 8.5 ns upper delta t cut</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF1AED9-2A40-3E4B-B414-28481040B7A7}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,6 +850,56 @@
         <v>0.309</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>-17.692699999999999</v>
+      </c>
+      <c r="C18">
+        <f>B18-B14</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>-17.821300000000001</v>
+      </c>
+      <c r="E18">
+        <f>D18-D14</f>
+        <v>9.9999999999766942E-5</v>
+      </c>
+      <c r="F18">
+        <v>2.5070000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.17299999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>-17.692799999999998</v>
+      </c>
+      <c r="C19">
+        <f>B19-B14</f>
+        <v>-9.9999999999766942E-5</v>
+      </c>
+      <c r="D19">
+        <v>-17.821400000000001</v>
+      </c>
+      <c r="E19">
+        <f>D19-D14</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2.2530000000000001</v>
+      </c>
+      <c r="G19">
+        <v>0.155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>